<commit_message>
Added the ability to override the regular CellReader
</commit_message>
<xml_diff>
--- a/src/test/resources/files/only_date.xlsx
+++ b/src/test/resources/files/only_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\example\src\test\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79889D91-3116-47D3-90BC-7914833ED602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239810AA-4573-4EF3-A60B-F373259ACEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -126,9 +126,9 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -349,8 +349,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -359,7 +359,7 @@
     <col min="2" max="2" width="31.265625" customWidth="1"/>
     <col min="3" max="3" width="33.265625" customWidth="1"/>
     <col min="4" max="4" width="34.73046875" customWidth="1"/>
-    <col min="5" max="5" width="19.1328125" customWidth="1"/>
+    <col min="5" max="5" width="34.06640625" customWidth="1"/>
     <col min="6" max="6" width="23.3984375" customWidth="1"/>
     <col min="7" max="7" width="20.3984375" customWidth="1"/>
   </cols>
@@ -377,7 +377,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -394,7 +394,7 @@
       <c r="D2" s="3">
         <v>46001</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>46001</v>
       </c>
       <c r="G2" s="4"/>
@@ -412,7 +412,7 @@
       <c r="D3" s="6">
         <v>45671</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>46002</v>
       </c>
       <c r="G3" s="4"/>
@@ -436,7 +436,7 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="D5" s="8">
+      <c r="D5" s="10">
         <v>45545.3</v>
       </c>
       <c r="E5" s="6"/>

</xml_diff>

<commit_message>
Refactoring and adding custom date format for LocalDateTime and OffsetDateTime
</commit_message>
<xml_diff>
--- a/src/test/resources/files/only_date.xlsx
+++ b/src/test/resources/files/only_date.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\example\src\test\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239810AA-4573-4EF3-A60B-F373259ACEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7474B92A-67D3-4A08-8540-A8849AFBC149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>offset_date_time_value</t>
   </si>
@@ -56,15 +56,38 @@
   </si>
   <si>
     <t>12/11/2025</t>
+  </si>
+  <si>
+    <t>custom_local_date_time_value_format</t>
+  </si>
+  <si>
+    <t>14-01-2022 13:00:12</t>
+  </si>
+  <si>
+    <t>15-01-2020 13:00:12</t>
+  </si>
+  <si>
+    <t>custom_offset_date_time_value_format</t>
+  </si>
+  <si>
+    <t>15 09 2025 15:40:37.180187 +02:00</t>
+  </si>
+  <si>
+    <t>15 09 2025 15:40:37.180187 Z</t>
+  </si>
+  <si>
+    <t>15 09 2025 15:40:37.180187 +05:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd"/>
     <numFmt numFmtId="168" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="170" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="172" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -117,18 +140,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -349,8 +374,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -360,8 +385,8 @@
     <col min="3" max="3" width="33.265625" customWidth="1"/>
     <col min="4" max="4" width="34.73046875" customWidth="1"/>
     <col min="5" max="5" width="34.06640625" customWidth="1"/>
-    <col min="6" max="6" width="23.3984375" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -377,8 +402,14 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>10</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -397,40 +428,50 @@
       <c r="E2" s="9">
         <v>46001</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="F2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>45671</v>
       </c>
       <c r="E3" s="9">
         <v>46002</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="F3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="4"/>
@@ -439,9 +480,14 @@
       <c r="D5" s="10">
         <v>45545.3</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="7" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>